<commit_message>
Update mics_dictionary_setcode.xlsx and mics_calculate.ado
</commit_message>
<xml_diff>
--- a/auxiliary_data/mics_dictionary_setcode.xlsx
+++ b/auxiliary_data/mics_dictionary_setcode.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="1" state="visible" r:id="rId2"/>
@@ -1539,19 +1539,20 @@
   </sheetPr>
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.4489795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4.45408163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="36.9897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.9081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2312,10 +2313,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2542,10 +2543,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2772,12 +2773,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="64" min="5" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="64" min="5" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2888,15 +2889,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="64" min="8" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="64" min="8" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3030,10 +3031,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3252,11 +3253,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="64" min="4" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="64" min="4" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3777,10 +3778,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4263,12 +4264,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="64" min="5" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="64" min="5" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7277,12 +7278,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="64" min="5" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="64" min="5" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10291,12 +10292,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="64" min="5" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="64" min="5" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13305,8 +13306,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="64" min="1" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="64" min="1" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13375,14 +13376,14 @@
   </sheetPr>
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A69" activeCellId="0" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13985,9 +13986,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.25"/>
-    <col collapsed="false" hidden="false" max="64" min="2" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="64" min="2" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14180,10 +14181,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14458,10 +14459,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14688,10 +14689,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14918,10 +14919,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15172,10 +15173,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15402,10 +15403,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="64" min="3" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>